<commit_message>
lab06: implement addValue() function
</commit_message>
<xml_diff>
--- a/Lab06/stack-trace.xlsx
+++ b/Lab06/stack-trace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeesmithh\repos\ceg3310-assignments\Lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774328A-8186-4728-9B66-EED3CA82314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE23414-C118-464B-80EA-2A595D508C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
   </bookViews>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE34279-D803-4DB1-874E-658A728EF49E}">
   <dimension ref="B1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lab06: implement printList() function
</commit_message>
<xml_diff>
--- a/Lab06/stack-trace.xlsx
+++ b/Lab06/stack-trace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeesmithh\repos\ceg3310-assignments\Lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE23414-C118-464B-80EA-2A595D508C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A196E691-4257-4F34-A706-E8BFD62CDBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>main() return address</t>
   </si>
@@ -1065,7 +1065,7 @@
   <dimension ref="B1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,9 +1913,7 @@
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="K24" s="2"/>
       <c r="L24" s="9"/>
       <c r="N24" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1955,9 +1953,6 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="L25" s="9"/>
       <c r="N25" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1997,9 +1992,7 @@
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="K26" s="2"/>
       <c r="L26" s="9"/>
       <c r="N26" s="5" t="str">
         <f t="shared" si="2"/>
@@ -2044,7 +2037,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="L27" s="9"/>
       <c r="N27" s="5" t="str">

</xml_diff>